<commit_message>
Add comments on detection file
</commit_message>
<xml_diff>
--- a/Load/ontology/Gates/GEMS/doc/non-raw_detection_gems.xlsx
+++ b/Load/ontology/Gates/GEMS/doc/non-raw_detection_gems.xlsx
@@ -1,34 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10412"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lindsabr\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezheng/Documents/EuPathDB-git/ApiCommonData/Load/ontology/Gates/GEMS/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5D08375-E387-43C1-8CA3-31BBF13402EC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE80636E-3915-1A46-B3C2-9239FCFFB4E3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1040" yWindow="460" windowWidth="20940" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="raw_detection_template" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="167">
   <si>
     <t>variable</t>
   </si>
@@ -543,6 +535,15 @@
   </si>
   <si>
     <t>Campylobacter coli</t>
+  </si>
+  <si>
+    <t>Should 1 be "ST"?</t>
+  </si>
+  <si>
+    <t>Aeromonus, typo?</t>
+  </si>
+  <si>
+    <t>JZ comments</t>
   </si>
 </sst>
 </file>
@@ -1034,10 +1035,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1395,16 +1400,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O65"/>
+  <dimension ref="A1:P65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="J11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3:XFD13"/>
+      <selection pane="bottomRight" activeCell="Q29" sqref="Q29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="15.5" style="2" customWidth="1"/>
@@ -1418,13 +1423,13 @@
     <col min="10" max="10" width="15.1640625" style="1" customWidth="1"/>
     <col min="11" max="11" width="22.6640625" style="1" customWidth="1"/>
     <col min="12" max="12" width="23.33203125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="31.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="31.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="30.33203125" style="2" customWidth="1"/>
     <col min="15" max="15" width="18.33203125" style="2" customWidth="1"/>
     <col min="16" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1467,8 +1472,11 @@
       <c r="O1" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" ht="93" x14ac:dyDescent="0.35">
+      <c r="P1" s="4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>20</v>
       </c>
@@ -1494,7 +1502,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>46</v>
       </c>
@@ -1534,7 +1542,7 @@
         <v>Virus in stool</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -1566,7 +1574,7 @@
         <v>Virus in stool</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>48</v>
       </c>
@@ -1582,7 +1590,7 @@
       <c r="E5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="3" t="s">
         <v>120</v>
       </c>
       <c r="M5" s="2" t="str">
@@ -1597,8 +1605,11 @@
         <f t="shared" si="2"/>
         <v>Bacteria in stool</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P5" s="3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>49</v>
       </c>
@@ -1630,7 +1641,7 @@
         <v>Virus in stool</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>50</v>
       </c>
@@ -1662,7 +1673,7 @@
         <v>Bacteria in stool</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>51</v>
       </c>
@@ -1694,7 +1705,7 @@
         <v>Bacteria in stool</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>52</v>
       </c>
@@ -1726,7 +1737,7 @@
         <v>Bacteria in stool</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>53</v>
       </c>
@@ -1758,7 +1769,7 @@
         <v>Bacteria in stool</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>54</v>
       </c>
@@ -1790,7 +1801,7 @@
         <v>Bacteria in stool</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>55</v>
       </c>
@@ -1822,7 +1833,7 @@
         <v>Eukaryota in stool</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>56</v>
       </c>
@@ -1854,7 +1865,7 @@
         <v>Eukaryota in stool</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>57</v>
       </c>
@@ -1898,7 +1909,7 @@
         <v>Bacteria in stool</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>58</v>
       </c>
@@ -1942,7 +1953,7 @@
         <v>Bacteria in stool</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>59</v>
       </c>
@@ -1983,7 +1994,7 @@
         <v>Bacteria in stool</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>60</v>
       </c>
@@ -2024,7 +2035,7 @@
         <v>Bacteria in stool</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>61</v>
       </c>
@@ -2062,7 +2073,7 @@
         <v>Bacteria in stool</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>62</v>
       </c>
@@ -2106,7 +2117,7 @@
         <v>Bacteria in stool</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>63</v>
       </c>
@@ -2147,7 +2158,7 @@
         <v>Bacteria in stool</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>64</v>
       </c>
@@ -2188,7 +2199,7 @@
         <v>Bacteria in stool</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>65</v>
       </c>
@@ -2223,7 +2234,7 @@
         <v>Bacteria in stool</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>66</v>
       </c>
@@ -2261,7 +2272,7 @@
         <v>Bacteria in stool</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>67</v>
       </c>
@@ -2305,7 +2316,7 @@
         <v>Bacteria in stool</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>68</v>
       </c>
@@ -2327,10 +2338,10 @@
       <c r="G25" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H25" s="1" t="s">
+      <c r="H25" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I25" s="1" t="s">
+      <c r="I25" s="3" t="s">
         <v>30</v>
       </c>
       <c r="J25" s="1" t="s">
@@ -2348,8 +2359,11 @@
         <f t="shared" si="2"/>
         <v>Bacteria in stool</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P25" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>69</v>
       </c>
@@ -2390,7 +2404,7 @@
         <v>Bacteria in stool</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>70</v>
       </c>
@@ -2430,8 +2444,9 @@
         <f t="shared" si="2"/>
         <v>Bacteria in stool</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P27" s="3"/>
+    </row>
+    <row r="28" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>71</v>
       </c>
@@ -2475,7 +2490,7 @@
         <v>Bacteria in stool</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>72</v>
       </c>
@@ -2519,7 +2534,7 @@
         <v>Bacteria in stool</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>73</v>
       </c>
@@ -2551,7 +2566,7 @@
         <v>Eukaryota in stool</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>74</v>
       </c>
@@ -2583,7 +2598,7 @@
         <v>Virus in stool</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>75</v>
       </c>
@@ -2615,7 +2630,7 @@
         <v>Virus in stool</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>76</v>
       </c>
@@ -2647,7 +2662,7 @@
         <v>Virus in stool</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>77</v>
       </c>
@@ -2679,7 +2694,7 @@
         <v>Virus in stool</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>78</v>
       </c>
@@ -2719,7 +2734,7 @@
         <v>Bacteria in stool</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>79</v>
       </c>
@@ -2751,7 +2766,7 @@
         <v>Bacteria in stool</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>80</v>
       </c>
@@ -2783,7 +2798,7 @@
         <v>Virus in stool</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>81</v>
       </c>
@@ -2815,7 +2830,7 @@
         <v>Bacteria in stool</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>82</v>
       </c>
@@ -2847,7 +2862,7 @@
         <v>Bacteria in stool</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>83</v>
       </c>
@@ -2879,7 +2894,7 @@
         <v>Bacteria in stool</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>84</v>
       </c>
@@ -2911,7 +2926,7 @@
         <v>Bacteria in stool</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>85</v>
       </c>
@@ -2943,7 +2958,7 @@
         <v>Bacteria in stool</v>
       </c>
     </row>
-    <row r="43" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>86</v>
       </c>
@@ -2975,7 +2990,7 @@
         <v>Bacteria in stool</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>87</v>
       </c>
@@ -3007,7 +3022,7 @@
         <v>Bacteria in stool</v>
       </c>
     </row>
-    <row r="45" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>88</v>
       </c>
@@ -3039,7 +3054,7 @@
         <v>Bacteria in stool</v>
       </c>
     </row>
-    <row r="46" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>89</v>
       </c>
@@ -3071,7 +3086,7 @@
         <v>Bacteria in stool</v>
       </c>
     </row>
-    <row r="47" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>90</v>
       </c>
@@ -3103,7 +3118,7 @@
         <v>Bacteria in stool</v>
       </c>
     </row>
-    <row r="48" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>91</v>
       </c>
@@ -3135,7 +3150,7 @@
         <v>Bacteria in stool</v>
       </c>
     </row>
-    <row r="49" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>92</v>
       </c>
@@ -3167,7 +3182,7 @@
         <v>Bacteria in stool</v>
       </c>
     </row>
-    <row r="50" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>93</v>
       </c>
@@ -3199,7 +3214,7 @@
         <v>Bacteria in stool</v>
       </c>
     </row>
-    <row r="51" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>94</v>
       </c>
@@ -3231,7 +3246,7 @@
         <v>Bacteria in stool</v>
       </c>
     </row>
-    <row r="52" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>95</v>
       </c>
@@ -3263,7 +3278,7 @@
         <v>Bacteria in stool</v>
       </c>
     </row>
-    <row r="53" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>96</v>
       </c>
@@ -3295,7 +3310,7 @@
         <v>Bacteria in stool</v>
       </c>
     </row>
-    <row r="54" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>97</v>
       </c>
@@ -3327,7 +3342,7 @@
         <v>Bacteria in stool</v>
       </c>
     </row>
-    <row r="55" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>98</v>
       </c>
@@ -3359,7 +3374,7 @@
         <v>Bacteria in stool</v>
       </c>
     </row>
-    <row r="56" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>99</v>
       </c>
@@ -3391,7 +3406,7 @@
         <v>Bacteria in stool</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>100</v>
       </c>
@@ -3431,7 +3446,7 @@
         <v>Bacteria in stool</v>
       </c>
     </row>
-    <row r="58" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>101</v>
       </c>
@@ -3463,7 +3478,7 @@
         <v>Bacteria in stool</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>102</v>
       </c>
@@ -3495,7 +3510,7 @@
         <v>Bacteria in stool</v>
       </c>
     </row>
-    <row r="60" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>103</v>
       </c>
@@ -3527,7 +3542,7 @@
         <v>Bacteria in stool</v>
       </c>
     </row>
-    <row r="61" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>104</v>
       </c>
@@ -3559,7 +3574,7 @@
         <v>Bacteria in stool</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>105</v>
       </c>
@@ -3591,7 +3606,7 @@
         <v>Bacteria in stool</v>
       </c>
     </row>
-    <row r="63" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>106</v>
       </c>
@@ -3623,7 +3638,7 @@
         <v>Bacteria in stool</v>
       </c>
     </row>
-    <row r="64" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>107</v>
       </c>
@@ -3655,7 +3670,7 @@
         <v>Bacteria in stool</v>
       </c>
     </row>
-    <row r="65" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>108</v>
       </c>

</xml_diff>